<commit_message>
feat:added support for new schema in admin side
</commit_message>
<xml_diff>
--- a/public/templates/Adynamics Question Template.xlsx
+++ b/public/templates/Adynamics Question Template.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>question_text</t>
   </si>
@@ -43,7 +43,7 @@
     <t>option_generation_rules</t>
   </si>
   <si>
-    <t>correct_answer_equation</t>
+    <t>no_of_times</t>
   </si>
   <si>
     <t>dynamic</t>
@@ -55,16 +55,37 @@
     <t>{"x": {"min": 1, "max": 10}, "y": {"min": 1, "max": 10}}</t>
   </si>
   <si>
-    <t>{"correct": "{x} + {y}", "wrong1": "{x} - {y}", "wrong2": "{x} * {y}", "wrong3": "{x} / {y}"}</t>
-  </si>
-  <si>
-    <t>x+y</t>
+    <t>{"correct": ["{x}+{y}","units"],"wrong1": ["{x} - {y}", "units"], "wrong2": ["{x} * {y}", "units"], "wrong3": ["{x} + {y} + 1", "units"]}</t>
   </si>
   <si>
     <t>What is the approximate compression of the Earth?</t>
   </si>
   <si>
     <t>static</t>
+  </si>
+  <si>
+    <t>dynamic conditional</t>
+  </si>
+  <si>
+    <t>Find Track (M)? If Track (T) is  {x}° and Variation is {y}°{direction}</t>
+  </si>
+  <si>
+    <t>{"range_values":{"x":{"min":0,"max":180},"y":{"min":0,"max":10}},"enum_values":{"direction":["W","E"]}}</t>
+  </si>
+  <si>
+    <t>{"direction === W":[{"correct":["x-y","units"],"wrong1":["{x} - {y} - 1","units"],"wrong2":["{x} * {y}","units"],"wrong3":["{x}+{y}","units"]}],"direction === E":[{"correct":["x+y","units"],"wrong1":["{x} + {y} + 1","units"],"wrong2":["{x} / {y}","units"],"wrong3":["{x}-{y}","units"]}]}</t>
+  </si>
+  <si>
+    <t>dynamic text conditional</t>
+  </si>
+  <si>
+    <t>What happens to Magnetic Compass when in the {hemisphere} Hemisphere and Accelerating in {direction} Direction?</t>
+  </si>
+  <si>
+    <t>{"hemisphere": ["Northern", "Southern"], "direction": ["North East","East"]}</t>
+  </si>
+  <si>
+    <t>{"hemisphere === Northern &amp;&amp; direction === North East":{"correct":"Apparent Turn to North Pole, Compass Turns Clockwise, Liquid Swirl increases error","wrong1":"Wrong Option 1","wrong2":"Wrong Option 2","wrong3":"Wrong Option 3"},"hemisphere === Northern &amp;&amp; direction === East":{"correct":"No error","wrong1":"Wrong Option 1","wrong2":"Wrong Option 2","wrong3":"Wrong Option 3"},"hemisphere === Southern &amp;&amp; direction === North East":{"correct":"Apparent Turn to South Pole, Compass Turns Anti Clockwise, Liquid Swirl increases error","wrong1":"Wrong Option 1","wrong2":"Wrong Option 2","wrong3":"Wrong Option 3"},"hemisphere === Southern &amp;&amp; direction === East":{"correct":"No error whatsover","wrong1":"Wrong Option 1","wrong2":"Wrong Option 2","wrong3":"Wrong Option 3"}}</t>
   </si>
 </sst>
 </file>
@@ -108,7 +129,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -132,6 +153,9 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="10" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -349,10 +373,9 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="8" max="8" width="14.63"/>
+    <col customWidth="1" min="8" max="8" width="20.88"/>
     <col customWidth="1" min="9" max="9" width="17.5"/>
-    <col customWidth="1" min="10" max="10" width="21.75"/>
-    <col customWidth="1" min="11" max="11" width="20.63"/>
+    <col customWidth="1" min="10" max="10" width="48.5"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -403,16 +426,16 @@
       <c r="J2" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="K2" s="2" t="s">
-        <v>15</v>
+      <c r="K2" s="1">
+        <v>3.0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>16</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>17</v>
       </c>
       <c r="C3" s="5">
         <v>0.03</v>
@@ -428,6 +451,43 @@
       </c>
       <c r="G3" s="1">
         <v>2.0</v>
+      </c>
+      <c r="K3" s="1">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="4" ht="147.75" customHeight="1">
+      <c r="B4" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H4" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="K4" s="1">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="B5" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="H5" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="I5" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="J5" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="K5" s="1">
+        <v>3.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>